<commit_message>
S'han afegit dos codis nous per el flagger
</commit_message>
<xml_diff>
--- a/output/GUIA MODELADO V2 2025-12-18 06-47-01_excel.xlsx
+++ b/output/GUIA MODELADO V2 2025-12-18 06-47-01_excel.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D510"/>
+  <dimension ref="A1:D511"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8160,7 +8160,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>141749</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
@@ -9584,14 +9584,10 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>54539</t>
-        </is>
-      </c>
-      <c r="C417" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>12613#</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr"/>
       <c r="D417" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -9606,7 +9602,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>378926#</t>
+          <t>349637#</t>
         </is>
       </c>
       <c r="C418" t="inlineStr"/>
@@ -9624,7 +9620,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>2008107#</t>
+          <t>f2d4f20de81b017428fb8429#</t>
         </is>
       </c>
       <c r="C419" t="inlineStr"/>
@@ -9642,10 +9638,14 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>2000023#</t>
-        </is>
-      </c>
-      <c r="C420" t="inlineStr"/>
+          <t>421251</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D420" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -9660,7 +9660,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>351049#</t>
+          <t>356146#</t>
         </is>
       </c>
       <c r="C421" t="inlineStr"/>
@@ -9678,7 +9678,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>Revit##0</t>
+          <t>2000920#</t>
         </is>
       </c>
       <c r="C422" t="inlineStr"/>
@@ -9696,7 +9696,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>368759#</t>
+          <t>360932#</t>
         </is>
       </c>
       <c r="C423" t="inlineStr"/>
@@ -9714,12 +9714,12 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>49561</t>
+          <t>416203</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>u</t>
+          <t>m2</t>
         </is>
       </c>
       <c r="D424" s="4" t="inlineStr">
@@ -9736,14 +9736,10 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>422357</t>
-        </is>
-      </c>
-      <c r="C425" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>351049#</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr"/>
       <c r="D425" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -9758,7 +9754,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>8c7cea80df2bffefc425b808#</t>
+          <t>2000126#</t>
         </is>
       </c>
       <c r="C426" t="inlineStr"/>
@@ -9776,10 +9772,14 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>2003100#</t>
-        </is>
-      </c>
-      <c r="C427" t="inlineStr"/>
+          <t>379821</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D427" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -9794,7 +9794,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>3b84c223c87cf9064f14146f#</t>
+          <t>378977#</t>
         </is>
       </c>
       <c r="C428" t="inlineStr"/>
@@ -9812,7 +9812,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>2003101#</t>
+          <t>2001320#</t>
         </is>
       </c>
       <c r="C429" t="inlineStr"/>
@@ -9830,10 +9830,14 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>68751ca122004bd195d41eb1#</t>
-        </is>
-      </c>
-      <c r="C430" t="inlineStr"/>
+          <t>400270</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
       <c r="D430" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -9848,14 +9852,10 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>422360</t>
-        </is>
-      </c>
-      <c r="C431" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>01763966511d36575635ed50#</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr"/>
       <c r="D431" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -9870,7 +9870,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>378959#</t>
+          <t>2c4e32d1964278dd07b2eda4#</t>
         </is>
       </c>
       <c r="C432" t="inlineStr"/>
@@ -9888,14 +9888,10 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>384768</t>
-        </is>
-      </c>
-      <c r="C433" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>68751ca122004bd195d41eb1#</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr"/>
       <c r="D433" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -9910,7 +9906,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>8482#</t>
+          <t>463aba37a91624c06d68e298#</t>
         </is>
       </c>
       <c r="C434" t="inlineStr"/>
@@ -9928,7 +9924,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>2000919#</t>
+          <t>355123#</t>
         </is>
       </c>
       <c r="C435" t="inlineStr"/>
@@ -9946,7 +9942,7 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>2001330#</t>
+          <t>2008107#</t>
         </is>
       </c>
       <c r="C436" t="inlineStr"/>
@@ -9964,14 +9960,10 @@
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>418400</t>
-        </is>
-      </c>
-      <c r="C437" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>Habit_PB#</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr"/>
       <c r="D437" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -9986,14 +9978,10 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>384444</t>
-        </is>
-      </c>
-      <c r="C438" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>d01be03cc289732a91b81be1#</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr"/>
       <c r="D438" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10008,10 +9996,14 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>2000171#</t>
-        </is>
-      </c>
-      <c r="C439" t="inlineStr"/>
+          <t>384444</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D439" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10026,7 +10018,7 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>cd56c8aa009fe005b32465f1#</t>
+          <t>3b84c223c87cf9064f14146f#</t>
         </is>
       </c>
       <c r="C440" t="inlineStr"/>
@@ -10044,7 +10036,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>2000032#</t>
+          <t>1bdb3e9f0abc22a9cab2723d#</t>
         </is>
       </c>
       <c r="C441" t="inlineStr"/>
@@ -10062,10 +10054,14 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>355123#</t>
-        </is>
-      </c>
-      <c r="C442" t="inlineStr"/>
+          <t>54539</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D442" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10080,7 +10076,7 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>2000160#</t>
+          <t>8482#</t>
         </is>
       </c>
       <c r="C443" t="inlineStr"/>
@@ -10098,14 +10094,10 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>137323</t>
-        </is>
-      </c>
-      <c r="C444" t="inlineStr">
-        <is>
-          <t>u</t>
-        </is>
-      </c>
+          <t>2003100#</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr"/>
       <c r="D444" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10120,7 +10112,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>ffa15592296ee41928620a0a#</t>
+          <t>cd56c8aa009fe005b32465f1#</t>
         </is>
       </c>
       <c r="C445" t="inlineStr"/>
@@ -10138,7 +10130,7 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>2000700#</t>
+          <t>2000032#</t>
         </is>
       </c>
       <c r="C446" t="inlineStr"/>
@@ -10174,7 +10166,7 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>416203</t>
+          <t>422357</t>
         </is>
       </c>
       <c r="C448" t="inlineStr">
@@ -10196,7 +10188,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>b74e94d46b2c057a14f47255#</t>
+          <t>2008163#</t>
         </is>
       </c>
       <c r="C449" t="inlineStr"/>
@@ -10214,7 +10206,7 @@
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>2000051#</t>
+          <t>Habit_P1#</t>
         </is>
       </c>
       <c r="C450" t="inlineStr"/>
@@ -10232,10 +10224,14 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>349637#</t>
-        </is>
-      </c>
-      <c r="C451" t="inlineStr"/>
+          <t>418400</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D451" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10250,10 +10246,14 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>c5d2dd0bf170338eeffbfdb5#</t>
-        </is>
-      </c>
-      <c r="C452" t="inlineStr"/>
+          <t>416213</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D452" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10268,7 +10268,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>12609#</t>
+          <t>2000011#</t>
         </is>
       </c>
       <c r="C453" t="inlineStr"/>
@@ -10286,7 +10286,7 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>356145#</t>
+          <t>b74e94d46b2c057a14f47255#</t>
         </is>
       </c>
       <c r="C454" t="inlineStr"/>
@@ -10304,10 +10304,14 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>2000920#</t>
-        </is>
-      </c>
-      <c r="C455" t="inlineStr"/>
+          <t>102462</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
       <c r="D455" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10340,7 +10344,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>356146#</t>
+          <t>395101#</t>
         </is>
       </c>
       <c r="C457" t="inlineStr"/>
@@ -10358,7 +10362,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>360932#</t>
+          <t>2000023#</t>
         </is>
       </c>
       <c r="C458" t="inlineStr"/>
@@ -10376,10 +10380,14 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>2000120#</t>
-        </is>
-      </c>
-      <c r="C459" t="inlineStr"/>
+          <t>423688</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D459" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10394,10 +10402,14 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>385031#</t>
-        </is>
-      </c>
-      <c r="C460" t="inlineStr"/>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>m3</t>
+        </is>
+      </c>
       <c r="D460" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10412,7 +10424,7 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>Áreas_PB#</t>
+          <t>2003200#</t>
         </is>
       </c>
       <c r="C461" t="inlineStr"/>
@@ -10430,7 +10442,7 @@
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>2000011#</t>
+          <t>2000051#</t>
         </is>
       </c>
       <c r="C462" t="inlineStr"/>
@@ -10448,10 +10460,14 @@
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>2001180#</t>
-        </is>
-      </c>
-      <c r="C463" t="inlineStr"/>
+          <t>141749</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
       <c r="D463" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10466,14 +10482,10 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>49504</t>
-        </is>
-      </c>
-      <c r="C464" t="inlineStr">
-        <is>
-          <t>u</t>
-        </is>
-      </c>
+          <t>356145#</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr"/>
       <c r="D464" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10488,10 +10500,14 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>2001263#</t>
-        </is>
-      </c>
-      <c r="C465" t="inlineStr"/>
+          <t>422360</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D465" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10506,7 +10522,7 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>416200</t>
+          <t>12615</t>
         </is>
       </c>
       <c r="C466" t="inlineStr">
@@ -10528,7 +10544,7 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>2001320#</t>
+          <t>2000120#</t>
         </is>
       </c>
       <c r="C467" t="inlineStr"/>
@@ -10546,7 +10562,7 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>2154006ce6da807a10c52529#</t>
+          <t>385031#</t>
         </is>
       </c>
       <c r="C468" t="inlineStr"/>
@@ -10564,10 +10580,14 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>12613#</t>
-        </is>
-      </c>
-      <c r="C469" t="inlineStr"/>
+          <t>423885</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D469" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10582,14 +10602,10 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>395062</t>
-        </is>
-      </c>
-      <c r="C470" t="inlineStr">
-        <is>
-          <t>u</t>
-        </is>
-      </c>
+          <t>378926#</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr"/>
       <c r="D470" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10604,7 +10620,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>Habit_PB#</t>
+          <t>88723c3731b7932f9f4568ac#</t>
         </is>
       </c>
       <c r="C471" t="inlineStr"/>
@@ -10622,10 +10638,14 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>2008163#</t>
-        </is>
-      </c>
-      <c r="C472" t="inlineStr"/>
+          <t>380816</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D472" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10640,7 +10660,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>88723c3731b7932f9f4568ac#</t>
+          <t>2001330#</t>
         </is>
       </c>
       <c r="C473" t="inlineStr"/>
@@ -10658,12 +10678,12 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>400270</t>
+          <t>421478</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>u</t>
+          <t>m2</t>
         </is>
       </c>
       <c r="D474" s="4" t="inlineStr">
@@ -10680,10 +10700,14 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>2003200#</t>
-        </is>
-      </c>
-      <c r="C475" t="inlineStr"/>
+          <t>Fill</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>m3</t>
+        </is>
+      </c>
       <c r="D475" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10698,7 +10722,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>354019#</t>
+          <t>151741#</t>
         </is>
       </c>
       <c r="C476" t="inlineStr"/>
@@ -10716,7 +10740,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>2001350#</t>
+          <t>2000160#</t>
         </is>
       </c>
       <c r="C477" t="inlineStr"/>
@@ -10734,14 +10758,10 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>102462</t>
-        </is>
-      </c>
-      <c r="C478" t="inlineStr">
-        <is>
-          <t>u</t>
-        </is>
-      </c>
+          <t>Revit##0</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr"/>
       <c r="D478" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10756,14 +10776,10 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>Fill</t>
-        </is>
-      </c>
-      <c r="C479" t="inlineStr">
-        <is>
-          <t>m3</t>
-        </is>
-      </c>
+          <t>2001300#</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr"/>
       <c r="D479" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10778,14 +10794,10 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>414195</t>
-        </is>
-      </c>
-      <c r="C480" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>378959#</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr"/>
       <c r="D480" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10800,10 +10812,14 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>2c4e32d1964278dd07b2eda4#</t>
-        </is>
-      </c>
-      <c r="C481" t="inlineStr"/>
+          <t>49561</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
       <c r="D481" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10818,7 +10834,7 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>378977#</t>
+          <t>2000170#</t>
         </is>
       </c>
       <c r="C482" t="inlineStr"/>
@@ -10836,14 +10852,10 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>416213</t>
-        </is>
-      </c>
-      <c r="C483" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>2001350#</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr"/>
       <c r="D483" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10858,7 +10870,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>2000035#</t>
+          <t>2000700#</t>
         </is>
       </c>
       <c r="C484" t="inlineStr"/>
@@ -10876,7 +10888,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>d01be03cc289732a91b81be1#</t>
+          <t>Áreas_P1#</t>
         </is>
       </c>
       <c r="C485" t="inlineStr"/>
@@ -10894,14 +10906,10 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>12615</t>
-        </is>
-      </c>
-      <c r="C486" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>2001180#</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr"/>
       <c r="D486" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10916,10 +10924,14 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>2000126#</t>
-        </is>
-      </c>
-      <c r="C487" t="inlineStr"/>
+          <t>416200</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D487" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10934,7 +10946,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>151741#</t>
+          <t>12609#</t>
         </is>
       </c>
       <c r="C488" t="inlineStr"/>
@@ -10970,10 +10982,14 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>2000170#</t>
-        </is>
-      </c>
-      <c r="C490" t="inlineStr"/>
+          <t>49504</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
       <c r="D490" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -10988,7 +11004,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>395101#</t>
+          <t>2001263#</t>
         </is>
       </c>
       <c r="C491" t="inlineStr"/>
@@ -11006,7 +11022,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>Habit_P1#</t>
+          <t>2000035#</t>
         </is>
       </c>
       <c r="C492" t="inlineStr"/>
@@ -11024,14 +11040,10 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>379821</t>
-        </is>
-      </c>
-      <c r="C493" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>2000996#</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr"/>
       <c r="D493" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11046,7 +11058,7 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>2000996#</t>
+          <t>3ac1d0acb7c1b37cfcba658e#</t>
         </is>
       </c>
       <c r="C494" t="inlineStr"/>
@@ -11064,14 +11076,10 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>416196</t>
-        </is>
-      </c>
-      <c r="C495" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>c5d2dd0bf170338eeffbfdb5#</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr"/>
       <c r="D495" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11086,10 +11094,14 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>463aba37a91624c06d68e298#</t>
-        </is>
-      </c>
-      <c r="C496" t="inlineStr"/>
+          <t>414195</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D496" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11104,14 +11116,10 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>380816</t>
-        </is>
-      </c>
-      <c r="C497" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>2003101#</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr"/>
       <c r="D497" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11126,7 +11134,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>Áreas_P1#</t>
+          <t>2000919#</t>
         </is>
       </c>
       <c r="C498" t="inlineStr"/>
@@ -11144,14 +11152,10 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>421478</t>
-        </is>
-      </c>
-      <c r="C499" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>8c7cea80df2bffefc425b808#</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr"/>
       <c r="D499" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11166,14 +11170,10 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>Cut</t>
-        </is>
-      </c>
-      <c r="C500" t="inlineStr">
-        <is>
-          <t>m3</t>
-        </is>
-      </c>
+          <t>73a5c388732eabc8da8068e5#</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr"/>
       <c r="D500" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11188,10 +11188,14 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>73a5c388732eabc8da8068e5#</t>
-        </is>
-      </c>
-      <c r="C501" t="inlineStr"/>
+          <t>384768</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D501" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11206,14 +11210,10 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>423885</t>
-        </is>
-      </c>
-      <c r="C502" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>354019#</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr"/>
       <c r="D502" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11228,14 +11228,10 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>423688</t>
-        </is>
-      </c>
-      <c r="C503" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>368759#</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr"/>
       <c r="D503" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11250,7 +11246,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>163904#</t>
+          <t>2000171#</t>
         </is>
       </c>
       <c r="C504" t="inlineStr"/>
@@ -11268,7 +11264,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>1bdb3e9f0abc22a9cab2723d#</t>
+          <t>163904#</t>
         </is>
       </c>
       <c r="C505" t="inlineStr"/>
@@ -11286,14 +11282,10 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>421251</t>
-        </is>
-      </c>
-      <c r="C506" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
+          <t>2154006ce6da807a10c52529#</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr"/>
       <c r="D506" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11308,10 +11300,14 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>f2d4f20de81b017428fb8429#</t>
-        </is>
-      </c>
-      <c r="C507" t="inlineStr"/>
+          <t>416196</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="D507" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11326,10 +11322,14 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>2001300#</t>
-        </is>
-      </c>
-      <c r="C508" t="inlineStr"/>
+          <t>395062</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
       <c r="D508" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11344,10 +11344,14 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>3ac1d0acb7c1b37cfcba658e#</t>
-        </is>
-      </c>
-      <c r="C509" t="inlineStr"/>
+          <t>137323</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
       <c r="D509" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
@@ -11362,11 +11366,29 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>01763966511d36575635ed50#</t>
+          <t>Áreas_PB#</t>
         </is>
       </c>
       <c r="C510" t="inlineStr"/>
       <c r="D510" s="4" t="inlineStr">
+        <is>
+          <t>AVÍS</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>NO MODELAT</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>ffa15592296ee41928620a0a#</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr"/>
+      <c r="D511" s="4" t="inlineStr">
         <is>
           <t>AVÍS</t>
         </is>
@@ -17439,7 +17461,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>141749</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">

</xml_diff>